<commit_message>
doc change, tasks week 3
</commit_message>
<xml_diff>
--- a/Documents/WeeklySchedule.xlsx
+++ b/Documents/WeeklySchedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name:</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Sate AI Tree/Deconstruct Pathfinding Demo/Sight cone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Francisco </t>
+  </si>
+  <si>
+    <t>Fixing issues with the pause menu, triggers and buttons</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:D8"/>
+  <dimension ref="A5:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,6 +415,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Shedules for Mocap and Weekly Shedule
</commit_message>
<xml_diff>
--- a/Documents/WeeklySchedule.xlsx
+++ b/Documents/WeeklySchedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name:</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Sate AI Tree/Deconstruct Pathfinding Demo/Sight cone</t>
+  </si>
+  <si>
+    <t>Emberlee</t>
+  </si>
+  <si>
+    <t>Do Mocap poses, think of things to code</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:D8"/>
+  <dimension ref="A5:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,6 +415,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added tasks for Austin and Chris for protype, Made a prefab for our temporary player controller
</commit_message>
<xml_diff>
--- a/Documents/WeeklySchedule.xlsx
+++ b/Documents/WeeklySchedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Name:</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>Do Mocap poses, think of things to code</t>
+  </si>
+  <si>
+    <t>Basic Networking, Basic Replication</t>
+  </si>
+  <si>
+    <t>PROTOTYPE</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Sounds</t>
   </si>
 </sst>
 </file>
@@ -87,12 +99,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -375,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:D10"/>
+  <dimension ref="A5:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,6 +455,32 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>42588</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new Week's task
</commit_message>
<xml_diff>
--- a/Documents/WeeklySchedule.xlsx
+++ b/Documents/WeeklySchedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Name:</t>
   </si>
@@ -45,9 +45,6 @@
     <t xml:space="preserve">Francisco </t>
   </si>
   <si>
-    <t>Fixing issues with the pause menu, triggers and buttons</t>
-  </si>
-  <si>
     <t>Emberlee</t>
   </si>
   <si>
@@ -64,6 +61,15 @@
   </si>
   <si>
     <t>Sounds</t>
+  </si>
+  <si>
+    <t>Francisco</t>
+  </si>
+  <si>
+    <t>Fixing issues with the pause menu, triggers and buttons.</t>
+  </si>
+  <si>
+    <t>Creating a new Player controller.</t>
   </si>
 </sst>
 </file>
@@ -393,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:D15"/>
+  <dimension ref="A5:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,20 +450,20 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
         <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -470,15 +476,23 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Emberlee added to Weekly Schedule
</commit_message>
<xml_diff>
--- a/Documents/WeeklySchedule.xlsx
+++ b/Documents/WeeklySchedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Name:</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Sounds</t>
+  </si>
+  <si>
+    <t>Create Mocap Poses and put them in unity</t>
   </si>
 </sst>
 </file>
@@ -393,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:D15"/>
+  <dimension ref="A5:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,6 +484,14 @@
         <v>14</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>